<commit_message>
:sparkles: Bundle make_ascii() to rebel()
</commit_message>
<xml_diff>
--- a/tests/testthat/fullwidth.xlsx
+++ b/tests/testthat/fullwidth.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="17560" yWindow="560" windowWidth="28800" windowHeight="17620" tabRatio="500"/>
+    <workbookView xWindow="29480" yWindow="840" windowWidth="28800" windowHeight="17620" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="42">
   <si>
     <t>１</t>
   </si>
@@ -470,6 +471,159 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
       <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>

</xml_diff>